<commit_message>
05월 19일자 UserDAO 정리
</commit_message>
<xml_diff>
--- a/0519~20 주말진행상황.xlsx
+++ b/0519~20 주말진행상황.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD4E5F15-A621-4C6A-9F3D-6FBA581FD9F6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{31220740-32D4-45DA-9541-3B66983EED99}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{9EA27C81-5605-4A34-9003-4C308B634538}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>UI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,24 +98,6 @@
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAO 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>session.select 의 결과를 바로 사용 불가. result type 맞춰서 변수에 대입 후 해당 변수를 사용해야.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserDAO.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String result = session.selectOne();
-result.equals() --&gt; (O)
-(String)(session.selectOne).equals() --&gt;(X)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -227,6 +209,60 @@
     <t>(미구현. 방법2로 구현할 계획)
 - 방법1. 경우의 수대로 UserVO 생성자 오버로딩
 - 방법2. 원래 값을 읽어와 VO에 1차 저장하고, 입력(수정)할 수 있는 모든 항목을 파라미터로 받아오되, 수정안한 항목을 null 체크를 통해 null이 아닌 경우에만 vo.setXXX() 를 통해 2차 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예외처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDAO.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(미구현)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 재확인 검사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null check로 결과 판단 시 sql문 select 대상 pw일 필요있나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(미수정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>try-catch-finally 블록에서 catch 내용 없음.
+CUD에서 if-else 구문에서 else 내용 없음.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회워가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탈퇴여부(status) 값 처리 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserVO.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(미수정)
+현재 가정. VO에는 status를 포함한 users 테이블의 모든 칼럼이 멤버 데이터로 들어가 있음. 사용자가 입력하지 않고 시스템적으로 탈퇴여부 값 전달한다고 가정함.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -251,15 +287,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -268,9 +310,43 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -282,23 +358,38 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,65 +706,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C493B5-24BC-44AA-825B-146CB36B2AAB}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="35.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="66.75" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="6">
         <v>43239</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>37</v>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -689,25 +780,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="280.5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>25</v>
+    <row r="4" spans="1:6" ht="264" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -723,72 +814,111 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>22</v>
+    </row>
+    <row r="7" spans="1:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="99" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="99" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>